<commit_message>
Adding report and styling
Committing my weekly report and adding styling to existing pages
</commit_message>
<xml_diff>
--- a/Weekly_Report.xlsx
+++ b/Weekly_Report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>WEEKLY REPORT</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Creation of welcome, sign_up and login page</t>
+  </si>
+  <si>
+    <t>14/05/2025</t>
+  </si>
+  <si>
+    <t>Creation of basic pages listed below the "Task" column but still to complete especially the styling aspect</t>
   </si>
 </sst>
 </file>
@@ -812,90 +821,66 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1433,157 +1418,146 @@
   <dimension ref="C1:J500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.9"/>
   <cols>
-    <col min="3" max="3" width="21" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.2222222222222" style="4" customWidth="1"/>
-    <col min="6" max="7" width="8.88888888888889" style="5"/>
-    <col min="8" max="8" width="21" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21" style="7" customWidth="1"/>
-    <col min="10" max="10" width="39.2222222222222" style="8" customWidth="1"/>
+    <col min="1" max="2" width="8.88888888888889" style="2"/>
+    <col min="3" max="3" width="21" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21" style="4" customWidth="1"/>
+    <col min="5" max="5" width="39.2222222222222" style="5" customWidth="1"/>
+    <col min="6" max="7" width="8.88888888888889" style="6"/>
+    <col min="8" max="8" width="21" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21" style="4" customWidth="1"/>
+    <col min="10" max="10" width="39.2222222222222" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.88888888888889" style="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="61" customHeight="1" spans="3:10">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="23"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" ht="52" customHeight="1" spans="3:10">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="11" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="H2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="31" customHeight="1" spans="3:10">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
+    <row r="4" ht="42" customHeight="1" spans="3:10">
+      <c r="C4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="27"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="27"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" ht="20.9" customHeight="1" spans="3:10">
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="27"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" ht="20.9" customHeight="1"/>
     <row r="14" ht="20.9" customHeight="1"/>

</xml_diff>